<commit_message>
Fix duplicate employeeId error during import
The unique index on employeeId was causing errors when:
1. Re-importing the same file (existing records)
2. Duplicates within the same Excel file

Fixed by:
- Deduplicating incoming data first (Map keeps last occurrence)
- Using existingMap to check if employeeId already exists in DB
- For existing: use put() with the existing internal id
- For new: use add() which auto-generates id

This ensures the unique index constraint is never violated.

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Upload2.xlsx
+++ b/Upload2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolajunser-richter/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolajunser-richter/workforce-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86DA43A-1CA7-AD4B-819A-4DA01303E98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FFABFB-F408-E949-B300-CD88F0510DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="1380" windowWidth="27840" windowHeight="16740" xr2:uid="{0E11C48F-CDB3-1349-A149-D43ED57ED975}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
   <si>
     <t>Position Code</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>1020-1802</t>
+  </si>
+  <si>
+    <t>11P001107895689</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <dimension ref="A1:AP5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,7 +1180,7 @@
         <v>84</v>
       </c>
       <c r="S5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="W5" s="1">
         <v>34478</v>

</xml_diff>